<commit_message>
Researching permissions, condensing file reading/writing functions
</commit_message>
<xml_diff>
--- a/Permissions.xlsx
+++ b/Permissions.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Code\Graduation-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D8FAD1C-B241-4A01-9626-9037A6F3849D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C26DED72-8E92-4BD5-B490-1C0FBB1814D3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="120" yWindow="60" windowWidth="20520" windowHeight="14910" activeTab="1" xr2:uid="{DB4C2691-3B4A-4A88-A677-245A38B64F20}"/>
+    <workbookView xWindow="28815" yWindow="60" windowWidth="11145" windowHeight="15315" activeTab="1" xr2:uid="{DB4C2691-3B4A-4A88-A677-245A38B64F20}"/>
   </bookViews>
   <sheets>
     <sheet name="Shared Permissions" sheetId="1" r:id="rId1"/>
     <sheet name="Permissions by Count" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="5" r:id="rId3"/>
+    <sheet name="Unique Permissions" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -35,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="575" uniqueCount="262">
   <si>
     <t>[1, dangerous]  android.permission.WRITE_CALENDAR</t>
   </si>
@@ -1187,10 +1189,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{57B450B2-1913-4CB7-AC96-0C309B5F4B82}">
-  <dimension ref="A1:C177"/>
+  <dimension ref="A1:C178"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C171" sqref="C171"/>
+    <sheetView topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="A86" sqref="A86"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1856,135 +1858,133 @@
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="2"/>
+      <c r="A81" s="1"/>
       <c r="B81" s="2"/>
+      <c r="C81" s="1"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
-        <v>60</v>
-      </c>
       <c r="B82" s="2"/>
-      <c r="C82" t="s">
-        <v>229</v>
-      </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" t="s">
-        <v>61</v>
+        <v>69</v>
       </c>
       <c r="B83" s="2"/>
       <c r="C83" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B84" s="2"/>
       <c r="C84" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B85" s="2"/>
       <c r="C85" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B86" s="2"/>
       <c r="C86" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B87" s="2"/>
       <c r="C87" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B88" s="2"/>
       <c r="C88" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B89" s="2"/>
       <c r="C89" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B90" s="2"/>
       <c r="C90" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B91" s="2"/>
       <c r="C91" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B92" s="2"/>
       <c r="C92" t="s">
-        <v>240</v>
+        <v>241</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B93" s="2"/>
       <c r="C93" t="s">
-        <v>243</v>
+        <v>240</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B94" s="2"/>
       <c r="C94" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B95" s="2"/>
+      <c r="C95" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B96" s="2"/>
       <c r="C96" t="s">
@@ -1993,505 +1993,511 @@
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A97" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B97" s="2"/>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A98" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B98" s="2"/>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A99" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B99" s="2"/>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A100" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="B100" s="2"/>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A101" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B101" s="2"/>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A102" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B102" s="2"/>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A103" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B103" s="2"/>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B104" s="2"/>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B105" s="2"/>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B106" s="2"/>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B107" s="2"/>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B108" s="2"/>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B109" s="2"/>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B110" s="2"/>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B111" s="2"/>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A112" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B112" s="2"/>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B113" s="2"/>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B114" s="2"/>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B115" s="2"/>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B116" s="2"/>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B117" s="2"/>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B118" s="2"/>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B119" s="2"/>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B120" s="2"/>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B121" s="2"/>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B122" s="2"/>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B123" s="2"/>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B124" s="2"/>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B125" s="2"/>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B126" s="2"/>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B127" s="2"/>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B128" s="2"/>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B129" s="2"/>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B130" s="2"/>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B131" s="2"/>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="B132" s="2"/>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B133" s="2"/>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B134" s="2"/>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B135" s="2"/>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B136" s="2"/>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B137" s="2"/>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B138" s="2"/>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B139" s="2"/>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B140" s="2"/>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B142" s="2"/>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B143" s="2"/>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B144" s="2"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B145" s="2"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B146" s="2"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B147" s="2"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B148" s="2"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B149" s="2"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B150" s="2"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B151" s="2"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B152" s="2"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B153" s="2"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A154" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B154" s="2"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B155" s="2"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B156" s="2"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="B157" s="2"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B158" s="2"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B160" s="2"/>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B161" s="2"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B162" s="2"/>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B163" s="2"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B164" s="2"/>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B165" s="2"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B166" s="2"/>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B167" s="2"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="B168" s="2"/>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B169" s="2"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B170" s="2"/>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
+        <v>154</v>
+      </c>
+      <c r="B171" s="2"/>
+    </row>
+    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A172" t="s">
         <v>155</v>
       </c>
-      <c r="B171" s="2"/>
-    </row>
-    <row r="172" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A172" s="1" t="s">
-        <v>151</v>
-      </c>
       <c r="B172" s="2"/>
-      <c r="C172" s="1" t="s">
-        <v>245</v>
-      </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>78</v>
+        <v>151</v>
       </c>
       <c r="B173" s="2"/>
       <c r="C173" s="1" t="s">
-        <v>78</v>
+        <v>245</v>
       </c>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>95</v>
+        <v>78</v>
       </c>
       <c r="B174" s="2"/>
       <c r="C174" s="1" t="s">
-        <v>231</v>
+        <v>78</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B175" s="2"/>
       <c r="C175" s="1" t="s">
-        <v>83</v>
+        <v>231</v>
       </c>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>113</v>
+        <v>83</v>
       </c>
       <c r="B176" s="2"/>
       <c r="C176" s="1" t="s">
-        <v>235</v>
+        <v>83</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>139</v>
+        <v>113</v>
       </c>
       <c r="B177" s="2"/>
       <c r="C177" s="1" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="178" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A178" s="1" t="s">
+        <v>139</v>
+      </c>
+      <c r="B178" s="2"/>
+      <c r="C178" s="1" t="s">
         <v>242</v>
       </c>
     </row>
@@ -2505,8 +2511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3E76CBB9-0C23-440C-AA8C-3D4EC8B9B527}">
   <dimension ref="A1:F177"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A65" workbookViewId="0">
-      <selection activeCell="C79" sqref="C79:C80"/>
+    <sheetView tabSelected="1" topLeftCell="A78" workbookViewId="0">
+      <selection activeCell="A85" sqref="A85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3225,7 +3231,7 @@
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="3" t="s">
-        <v>62</v>
+        <v>76</v>
       </c>
       <c r="C98" s="3" t="s">
         <v>241</v>
@@ -3233,76 +3239,76 @@
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="3" t="s">
-        <v>67</v>
+        <v>71</v>
       </c>
       <c r="C99" s="3" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="3" t="s">
-        <v>71</v>
+      <c r="A100" t="s">
+        <v>95</v>
       </c>
       <c r="C100" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="3" t="s">
-        <v>76</v>
+      <c r="A101" t="s">
+        <v>127</v>
       </c>
       <c r="C101" s="3" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
-        <v>83</v>
+      <c r="A102" s="3" t="s">
+        <v>62</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>91</v>
+      <c r="A103" s="3" t="s">
+        <v>67</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" t="s">
-        <v>95</v>
+        <v>128</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" t="s">
-        <v>106</v>
+        <v>148</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" t="s">
-        <v>123</v>
+        <v>83</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" t="s">
-        <v>128</v>
+        <v>106</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" t="s">
-        <v>130</v>
+        <v>91</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" t="s">
-        <v>148</v>
+        <v>130</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" t="s">
-        <v>63</v>
+        <v>93</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
@@ -3312,207 +3318,207 @@
     </row>
     <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" t="s">
-        <v>65</v>
+        <v>155</v>
       </c>
     </row>
     <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" t="s">
-        <v>66</v>
+        <v>94</v>
       </c>
     </row>
     <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>68</v>
+        <v>142</v>
       </c>
     </row>
     <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" t="s">
-        <v>70</v>
+        <v>63</v>
       </c>
     </row>
     <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" t="s">
-        <v>72</v>
+        <v>82</v>
       </c>
     </row>
     <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" t="s">
-        <v>73</v>
+        <v>153</v>
       </c>
     </row>
     <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" t="s">
-        <v>74</v>
+        <v>108</v>
       </c>
     </row>
     <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" t="s">
-        <v>75</v>
+        <v>118</v>
       </c>
     </row>
     <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" t="s">
-        <v>77</v>
+        <v>116</v>
       </c>
     </row>
     <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" t="s">
-        <v>79</v>
+        <v>96</v>
       </c>
     </row>
     <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" t="s">
-        <v>81</v>
+        <v>154</v>
       </c>
     </row>
     <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" t="s">
-        <v>82</v>
+        <v>104</v>
       </c>
     </row>
     <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" t="s">
-        <v>85</v>
+        <v>141</v>
       </c>
     </row>
     <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" t="s">
-        <v>88</v>
+        <v>117</v>
       </c>
     </row>
     <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" t="s">
-        <v>89</v>
+        <v>136</v>
       </c>
     </row>
     <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" t="s">
-        <v>92</v>
+        <v>125</v>
       </c>
     </row>
     <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>93</v>
+        <v>60</v>
       </c>
     </row>
     <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" t="s">
-        <v>94</v>
+        <v>81</v>
       </c>
     </row>
     <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
     </row>
     <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" t="s">
-        <v>97</v>
+        <v>140</v>
       </c>
     </row>
     <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
     </row>
     <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" t="s">
-        <v>100</v>
+        <v>73</v>
       </c>
     </row>
     <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" t="s">
-        <v>101</v>
+        <v>144</v>
       </c>
     </row>
     <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" t="s">
-        <v>103</v>
+        <v>79</v>
       </c>
     </row>
     <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
     </row>
     <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" t="s">
-        <v>105</v>
+        <v>131</v>
       </c>
     </row>
     <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" t="s">
-        <v>107</v>
+        <v>88</v>
       </c>
     </row>
     <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" t="s">
-        <v>108</v>
+        <v>90</v>
       </c>
     </row>
     <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" t="s">
-        <v>109</v>
+        <v>74</v>
       </c>
     </row>
     <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" t="s">
-        <v>110</v>
+        <v>145</v>
       </c>
     </row>
     <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" t="s">
-        <v>111</v>
+        <v>61</v>
       </c>
     </row>
     <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" t="s">
-        <v>112</v>
+        <v>85</v>
       </c>
     </row>
     <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
     </row>
     <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
     </row>
     <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" t="s">
-        <v>117</v>
+        <v>121</v>
       </c>
     </row>
     <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
     </row>
     <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" t="s">
-        <v>119</v>
+        <v>77</v>
       </c>
     </row>
     <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" t="s">
-        <v>60</v>
+        <v>112</v>
       </c>
     </row>
     <row r="153" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A153" t="s">
-        <v>61</v>
+        <v>143</v>
       </c>
     </row>
     <row r="154" spans="1:1" x14ac:dyDescent="0.25">
@@ -3522,117 +3528,446 @@
     </row>
     <row r="155" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A155" t="s">
-        <v>131</v>
+        <v>120</v>
       </c>
     </row>
     <row r="156" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A156" t="s">
-        <v>133</v>
+        <v>98</v>
       </c>
     </row>
     <row r="157" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A157" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
     </row>
     <row r="158" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A158" t="s">
-        <v>136</v>
+        <v>89</v>
       </c>
     </row>
     <row r="159" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A159" t="s">
-        <v>138</v>
+        <v>65</v>
       </c>
     </row>
     <row r="160" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A160" t="s">
-        <v>140</v>
+        <v>150</v>
       </c>
     </row>
     <row r="161" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A161" t="s">
-        <v>141</v>
+        <v>107</v>
       </c>
     </row>
     <row r="162" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A162" t="s">
-        <v>142</v>
+        <v>105</v>
       </c>
     </row>
     <row r="163" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A163" t="s">
-        <v>143</v>
+        <v>70</v>
       </c>
     </row>
     <row r="164" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A164" t="s">
-        <v>144</v>
+        <v>119</v>
       </c>
     </row>
     <row r="165" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A165" t="s">
-        <v>145</v>
+        <v>109</v>
       </c>
     </row>
     <row r="166" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A166" t="s">
-        <v>146</v>
+        <v>129</v>
       </c>
     </row>
     <row r="167" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A167" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="168" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A168" t="s">
-        <v>150</v>
+        <v>103</v>
       </c>
     </row>
     <row r="169" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A169" t="s">
-        <v>153</v>
+        <v>66</v>
       </c>
     </row>
     <row r="170" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A170" t="s">
-        <v>154</v>
+        <v>72</v>
       </c>
     </row>
     <row r="171" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A171" t="s">
-        <v>155</v>
+        <v>110</v>
       </c>
     </row>
     <row r="172" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A172" t="s">
-        <v>129</v>
+        <v>133</v>
       </c>
     </row>
     <row r="173" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A173" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
     </row>
     <row r="174" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A174" t="s">
-        <v>125</v>
+        <v>149</v>
       </c>
     </row>
     <row r="175" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A175" t="s">
-        <v>120</v>
+        <v>97</v>
       </c>
     </row>
     <row r="176" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A176" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
     </row>
     <row r="177" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A177" t="s">
-        <v>122</v>
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{79271F26-580F-42F1-8CCA-E516449247F9}">
+  <dimension ref="A1:A15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="94.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>239</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:A68">
+    <sortCondition ref="A1:A68"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2627E15-E98E-44B9-959C-B08E1638BECB}">
+  <dimension ref="A1:C35"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C36" sqref="C36"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="72.5703125" customWidth="1"/>
+    <col min="2" max="2" width="1.140625" customWidth="1"/>
+    <col min="3" max="3" width="70.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>247</v>
+      </c>
+      <c r="C1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>257</v>
+      </c>
+      <c r="C2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>259</v>
+      </c>
+      <c r="C3" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>260</v>
+      </c>
+      <c r="C4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C5" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>40</v>
+      </c>
+      <c r="C7" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>27</v>
+      </c>
+      <c r="C8" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>44</v>
+      </c>
+      <c r="C9" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>45</v>
+      </c>
+      <c r="C10" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>49</v>
+      </c>
+      <c r="C12" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>46</v>
+      </c>
+      <c r="C15" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>39</v>
+      </c>
+      <c r="C16" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C17" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C18" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>58</v>
+      </c>
+      <c r="C20" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C22" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C23" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C25" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C26" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C27" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C28" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C30" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C31" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C32" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="33" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C33" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="34" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C34" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="35" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C35" t="s">
+        <v>218</v>
       </c>
     </row>
   </sheetData>

</xml_diff>